<commit_message>
Asiagancion de trabajo de base de datos
</commit_message>
<xml_diff>
--- a/tablasMultiplataforma.xlsx
+++ b/tablasMultiplataforma.xlsx
@@ -83,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A13" authorId="0" shapeId="0">
+    <comment ref="A14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,55 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0">
+    <comment ref="J14" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Los servcicios solo llevan id nombre y precio de venta</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G17" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>USER:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Productos varios solo lleva id nombre marca existencia precio de venta y de compra.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -131,31 +179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>USER:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Los servcicios solo llevan id nombre y precio de venta</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B25" authorId="0" shapeId="0">
+    <comment ref="B21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -179,7 +203,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A27" authorId="0" shapeId="0">
+    <comment ref="H23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -199,7 +223,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Productos varios solo lleva id nombre marca existencia precio de venta y de compra.</t>
+Falta nombre del producto</t>
         </r>
       </text>
     </comment>
@@ -228,36 +252,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="B33" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>USER:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Falta nombre del producto</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
   <si>
     <t>producto</t>
   </si>
@@ -452,6 +452,18 @@
   </si>
   <si>
     <t>Detalle</t>
+  </si>
+  <si>
+    <t>Jennifer</t>
+  </si>
+  <si>
+    <t>Kattia</t>
+  </si>
+  <si>
+    <t>Diego</t>
+  </si>
+  <si>
+    <t>Carlos</t>
   </si>
 </sst>
 </file>
@@ -559,7 +571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -591,6 +603,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -606,6 +624,515 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectángulo 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="142875"/>
+          <a:ext cx="2219325" cy="4105275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-HN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rectángulo 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2809874" y="114299"/>
+          <a:ext cx="1914525" cy="3457575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-HN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectángulo 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5210174" y="76199"/>
+          <a:ext cx="2295526" cy="4391026"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-HN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectángulo 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8020050" y="57150"/>
+          <a:ext cx="2381250" cy="3343275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-HN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectángulo 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8010525" y="3524250"/>
+          <a:ext cx="2381250" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-HN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectángulo 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2790825" y="3733800"/>
+          <a:ext cx="1962150" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-HN" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Rectángulo 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="4333875"/>
+          <a:ext cx="2228850" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-HN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>685799</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Rectángulo 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5238749" y="4533900"/>
+          <a:ext cx="2257425" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="57150">
+          <a:solidFill>
+            <a:schemeClr val="tx1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="es-HN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -905,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:K33"/>
+  <dimension ref="A2:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,10 +1688,6 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="7"/>
       <c r="D13" s="3" t="s">
         <v>56</v>
       </c>
@@ -1177,12 +1700,10 @@
       <c r="H13" s="9"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7"/>
       <c r="D14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1195,13 +1716,17 @@
       <c r="H14" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="J14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>8</v>
+      <c r="A15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>57</v>
@@ -1215,10 +1740,16 @@
       <c r="H15" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>8</v>
@@ -1229,10 +1760,16 @@
       <c r="E16" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>8</v>
@@ -1243,13 +1780,23 @@
       <c r="E17" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>2</v>
+      <c r="G17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="7"/>
+      <c r="J17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>61</v>
@@ -1257,113 +1804,100 @@
       <c r="E18" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="G20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K20" s="13"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B23" s="1" t="s">
+      <c r="D21" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="14"/>
+      <c r="G21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="G22" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G23" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="H23" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="13"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="G25:H25"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="J2:K2"/>
@@ -1373,6 +1907,7 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>